<commit_message>
added blank excel file
</commit_message>
<xml_diff>
--- a/docs/schedule.xlsx
+++ b/docs/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\PythonProjects\autozoomer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444A3E26-6942-43A7-AC24-4C74F6FE76B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905A39E7-C035-4F75-9B7C-4312E9223B5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Class Name</t>
   </si>
@@ -70,33 +70,6 @@
   </si>
   <si>
     <t>Open application Link</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>https://oregonstate.zoom.us/j/95802901043?pwd=U2NxZzVRY0VYay8rRjRyQkJGNWxKZz09&amp;uname=James+Wilcock#success</t>
-  </si>
-  <si>
-    <t>WR 327</t>
-  </si>
-  <si>
-    <t>https://oregonstate.zoom.us/j/94114941355?pwd=VFZpUjBGNWoyT0tCR0FqSkR6WmpzQT09&amp;uname=James+Wilcock#success</t>
-  </si>
-  <si>
-    <t>ENGR 202</t>
-  </si>
-  <si>
-    <t>https://oregonstate.zoom.us/j/91672454319?pwd=RGJQcjNNWmtPcTEvMjN1WEw2QzB0UT09</t>
-  </si>
-  <si>
-    <t>ED 216</t>
-  </si>
-  <si>
-    <t>https://oregonstate.zoom.us/j/93753891197?pwd=K1hUVi96UTdhR0xGMWdGbjdKdTY4dz09</t>
-  </si>
-  <si>
-    <t>AG 301</t>
   </si>
 </sst>
 </file>
@@ -474,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H2" sqref="A2:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -534,73 +507,21 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.49791666666666662</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="D2" s="1"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.37291666666666662</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
+      <c r="B3" s="4"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.4145833333333333</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
+      <c r="B4" s="4"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.6645833333333333</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
+      <c r="B5" s="4"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
@@ -912,13 +833,8 @@
       <c r="D107" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" location="success" xr:uid="{8CA08CBE-52E8-459E-A499-946FD75FF64F}"/>
-    <hyperlink ref="B4" r:id="rId2" tooltip="https://oregonstate.zoom.us/j/91672454319?pwd=RGJQcjNNWmtPcTEvMjN1WEw2QzB0UT09" xr:uid="{16D8D6D1-17D2-4267-A419-E685D59F51A0}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{0130BD92-3F17-4D35-9A22-40E930AF2BB1}"/>
-  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>